<commit_message>
Add dealerName field to the payment entity
</commit_message>
<xml_diff>
--- a/src/test/resources/files/payment.xlsx
+++ b/src/test/resources/files/payment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>description</t>
   </si>
@@ -193,6 +193,48 @@
   </si>
   <si>
     <t>paymentNumber13</t>
+  </si>
+  <si>
+    <t>dealerName</t>
+  </si>
+  <si>
+    <t>dealerName1</t>
+  </si>
+  <si>
+    <t>dealerName2</t>
+  </si>
+  <si>
+    <t>dealerName3</t>
+  </si>
+  <si>
+    <t>dealerName4</t>
+  </si>
+  <si>
+    <t>dealerName5</t>
+  </si>
+  <si>
+    <t>dealerName6</t>
+  </si>
+  <si>
+    <t>dealerName7</t>
+  </si>
+  <si>
+    <t>dealerName8</t>
+  </si>
+  <si>
+    <t>dealerName9</t>
+  </si>
+  <si>
+    <t>dealerName10</t>
+  </si>
+  <si>
+    <t>dealerName11</t>
+  </si>
+  <si>
+    <t>dealerName12</t>
+  </si>
+  <si>
+    <t>dealerName13</t>
   </si>
 </sst>
 </file>
@@ -532,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +586,7 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -563,8 +605,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -583,8 +628,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -603,8 +651,11 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -623,8 +674,11 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -643,8 +697,11 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -663,8 +720,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -683,8 +743,11 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -703,8 +766,11 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -723,8 +789,11 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -743,8 +812,11 @@
       <c r="F10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -763,8 +835,11 @@
       <c r="F11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -783,8 +858,11 @@
       <c r="F12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -803,8 +881,11 @@
       <c r="F13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -822,6 +903,9 @@
       </c>
       <c r="F14" t="s">
         <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include purchase-order-number in the payment properties
</commit_message>
<xml_diff>
--- a/src/test/resources/files/payment.xlsx
+++ b/src/test/resources/files/payment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>description</t>
   </si>
@@ -235,6 +235,48 @@
   </si>
   <si>
     <t>dealerName13</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber1</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber2</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber3</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber4</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber5</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber6</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber7</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber8</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber9</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber10</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber11</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber12</t>
+  </si>
+  <si>
+    <t>purchaseOrderNumber13</t>
   </si>
 </sst>
 </file>
@@ -574,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +628,7 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -608,8 +650,11 @@
       <c r="G1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -631,8 +676,11 @@
       <c r="G2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -654,8 +702,11 @@
       <c r="G3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -677,8 +728,11 @@
       <c r="G4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -700,8 +754,11 @@
       <c r="G5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -723,8 +780,11 @@
       <c r="G6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -746,8 +806,11 @@
       <c r="G7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -769,8 +832,11 @@
       <c r="G8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -792,8 +858,11 @@
       <c r="G9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -815,8 +884,11 @@
       <c r="G10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -838,8 +910,11 @@
       <c r="G11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -861,8 +936,11 @@
       <c r="G12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -884,8 +962,11 @@
       <c r="G13" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -906,6 +987,9 @@
       </c>
       <c r="G14" t="s">
         <v>71</v>
+      </c>
+      <c r="H14" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>